<commit_message>
Ajust do backlog e criação de User Storie
</commit_message>
<xml_diff>
--- a/Análise de Sistemas/PBC - Product Backlog Classified V2.xlsx
+++ b/Análise de Sistemas/PBC - Product Backlog Classified V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme.bispo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.nascimento\Desktop\Grupo_04-2ADSA\Análise de Sistemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F6500C-F4E2-48E2-BAEB-437D61592047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C551E9CD-9A1F-4805-82FE-C5686B25EE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36810" yWindow="4215" windowWidth="12300" windowHeight="6150" tabRatio="350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>João</t>
   </si>
@@ -268,6 +268,18 @@
   </si>
   <si>
     <t>A aplicação deverá monitorar o hardware das máquinas e mostrar as informações em uma DASHBOARD (SITE).</t>
+  </si>
+  <si>
+    <t>US#05 &lt;Verificação de transação&gt;</t>
+  </si>
+  <si>
+    <t>Realizar a verificação do sistema para saber se existe alguma transação em andamento no momento em que o totem estiver ligado.</t>
+  </si>
+  <si>
+    <t>US#06 &lt;Abertura automatica do programa&gt;</t>
+  </si>
+  <si>
+    <t>Após a reinicialização do sistema, os softwares necessarios para compras futuas devem ser iniciados de maneira automatica.</t>
   </si>
 </sst>
 </file>
@@ -601,7 +613,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -734,6 +746,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -743,7 +756,10 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="20" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
@@ -1012,9 +1028,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>963996</xdr:colOff>
+      <xdr:colOff>971616</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>918881</xdr:rowOff>
+      <xdr:rowOff>934121</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1358,7 +1374,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
-            <a:t>#01 Eu como técnico gostaria que eu fosse avisado por mensagem quando uma máquina atingisse um nível elevado de consumo de hardware durante um tempo prolongado.</a:t>
+            <a:t>#XX Eu como técnico gostaria que eu fosse avisado por mensagem quando uma máquina atingisse um nível elevado de consumo de hardware durante um tempo prolongado.</a:t>
           </a:r>
           <a:endParaRPr lang="pt-BR" sz="1800"/>
         </a:p>
@@ -1433,7 +1449,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
-            <a:t>#02 Eu como gerente do estabelecimento quero que tenha um sistema que monitore o consumo de hardware das máquinas e me mostre de forma gráfica a situação atual das mesmas.</a:t>
+            <a:t>#01 Eu como gerente do estabelecimento quero que tenha um sistema que monitore o consumo de hardware das máquinas e me mostre de forma gráfica a situação atual das mesmas.</a:t>
           </a:r>
           <a:endParaRPr lang="pt-BR" sz="1800"/>
         </a:p>
@@ -1502,6 +1518,52 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>US#05</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Eu como técnico quero poder monitorar se existe alguma transação no momento, para que no momento em que for realizada alguma ação, não interfira na compra do cliente.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="pt-BR" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -1571,11 +1633,11 @@
         <a:p>
           <a:r>
             <a:rPr lang="pt-BR" sz="1800"/>
-            <a:t>US#03</a:t>
+            <a:t>US#02</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
-            <a:t> Eu como técnico quero que tenha uma funcionalidade que possibilite com que eu reinicie a máquina quando julgar necessário</a:t>
+            <a:t> Eu como técnico quero que exista uma dashboard em meu software com inuito de visualização das informações que foram coletadas</a:t>
           </a:r>
           <a:endParaRPr lang="pt-BR" sz="1800"/>
         </a:p>
@@ -1644,6 +1706,52 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>US#04</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Eu como técnico quero que o cache da máquina seja limpo quando o uso de processamento permaneça em um nível elevado durante um tempo prolongado.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="pt-BR" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -1713,12 +1821,247 @@
         <a:p>
           <a:r>
             <a:rPr lang="pt-BR" sz="1800"/>
-            <a:t>US#04</a:t>
+            <a:t>US#03</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
-            <a:t> Eu como técnico quero que o cache da máquina seja limpo quando o uso de processamento permaneça em um nível elevado durante um tempo prolongado.</a:t>
+            <a:t> Eu como técnico quero poder reinicializar a maquina quando achar necessario para evitar problemas nos totens.</a:t>
           </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>173144</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>58632</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="CaixaDeTexto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{392FA5B2-E535-41EC-B891-3AD43AEC1B21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10163811" y="58632"/>
+          <a:ext cx="5869939" cy="1391285"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>US#06</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Eu como técnico quero que meu programa tenha a capacidade de realizar a abertura dos programas necessarios quando estiver inicializando para que o processo seja automatizado, sem necessidade de um técnico.</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>173144</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38643</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="CaixaDeTexto 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62134852-DE0A-4575-A3AC-F1C268A047AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10163811" y="1520189"/>
+          <a:ext cx="5859356" cy="1397121"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800"/>
+            <a:t>US#07</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
+            <a:t> Eu como técnico que meu programa tenha a capacidade de realizar a abertura dos programas necessarios para que n</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>178012</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>143420</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="CaixaDeTexto 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3510663-E886-4D72-9DC6-F19499EF71D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10168679" y="2970107"/>
+          <a:ext cx="5886238" cy="1406646"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
           <a:endParaRPr lang="pt-BR" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -2052,41 +2395,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:K41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.28515625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="0.7109375" style="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="14"/>
-    <col min="11" max="11" width="13.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="14"/>
+    <col min="1" max="1" width="1.5546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="73.44140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="0.6640625" style="16" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="14"/>
+    <col min="11" max="11" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="8.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:11" ht="89.25" customHeight="1" thickBot="1">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
-    </row>
-    <row r="3" spans="2:11" ht="9.9499999999999993" customHeight="1" thickBot="1"/>
-    <row r="4" spans="2:11" s="20" customFormat="1" ht="24.95" customHeight="1" thickBot="1">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
+    </row>
+    <row r="3" spans="2:11" ht="9.9" customHeight="1" thickBot="1"/>
+    <row r="4" spans="2:11" s="20" customFormat="1" ht="24.9" customHeight="1" thickBot="1">
       <c r="B4" s="33" t="s">
         <v>23</v>
       </c>
@@ -2112,7 +2455,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="24" customFormat="1" ht="45.75" thickBot="1">
+    <row r="5" spans="2:11" s="24" customFormat="1" ht="29.4" thickBot="1">
       <c r="B5" s="39" t="s">
         <v>21</v>
       </c>
@@ -2148,7 +2491,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="2:11" s="24" customFormat="1" ht="30.75" thickBot="1">
+    <row r="7" spans="2:11" s="24" customFormat="1" ht="29.4" thickBot="1">
       <c r="B7" s="39" t="s">
         <v>21</v>
       </c>
@@ -2168,7 +2511,7 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
     </row>
-    <row r="8" spans="2:11" s="24" customFormat="1" ht="45.75" thickBot="1">
+    <row r="8" spans="2:11" s="24" customFormat="1" ht="43.8" thickBot="1">
       <c r="B8" s="39" t="s">
         <v>21</v>
       </c>
@@ -2186,7 +2529,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
     </row>
-    <row r="9" spans="2:11" s="24" customFormat="1" ht="30.75" thickBot="1">
+    <row r="9" spans="2:11" s="24" customFormat="1" ht="29.4" thickBot="1">
       <c r="B9" s="39" t="s">
         <v>21</v>
       </c>
@@ -2204,28 +2547,40 @@
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
     </row>
-    <row r="10" spans="2:11" s="24" customFormat="1" ht="15.75" thickBot="1">
+    <row r="10" spans="2:11" s="24" customFormat="1" ht="45" customHeight="1" thickBot="1">
       <c r="B10" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="37"/>
+      <c r="C10" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>63</v>
+      </c>
       <c r="E10" s="25"/>
-      <c r="F10" s="23"/>
+      <c r="F10" s="23" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
     </row>
-    <row r="11" spans="2:11" s="24" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="11" spans="2:11" s="24" customFormat="1" ht="49.2" customHeight="1" thickBot="1">
       <c r="B11" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="38"/>
+      <c r="C11" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>65</v>
+      </c>
       <c r="E11" s="25"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="H11" s="23" t="s">
+        <v>17</v>
+      </c>
       <c r="I11" s="23"/>
     </row>
     <row r="12" spans="2:11" s="24" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
@@ -2565,14 +2920,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="52.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="52.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1">
@@ -2677,7 +3034,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="23.25">
+    <row r="17" spans="1:2" ht="23.4">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
@@ -2685,7 +3042,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="23.25">
+    <row r="18" spans="1:2" ht="23.4">
       <c r="A18" s="11" t="s">
         <v>26</v>
       </c>
@@ -2693,7 +3050,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23.25">
+    <row r="19" spans="1:2" ht="23.4">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -2701,7 +3058,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="23.25">
+    <row r="20" spans="1:2" ht="23.4">
       <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
@@ -2709,7 +3066,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="23.25">
+    <row r="21" spans="1:2" ht="23.4">
       <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
@@ -2717,7 +3074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="23.25">
+    <row r="22" spans="1:2" ht="23.4">
       <c r="A22" s="11" t="s">
         <v>30</v>
       </c>
@@ -2725,7 +3082,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="23.25">
+    <row r="23" spans="1:2" ht="23.4">
       <c r="A23" s="11" t="s">
         <v>31</v>
       </c>
@@ -2733,7 +3090,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="23.25">
+    <row r="24" spans="1:2" ht="23.4">
       <c r="A24" s="11" t="s">
         <v>32</v>
       </c>
@@ -2741,7 +3098,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="23.25">
+    <row r="25" spans="1:2" ht="23.4">
       <c r="A25" s="11" t="s">
         <v>33</v>
       </c>
@@ -2749,7 +3106,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="23.25">
+    <row r="26" spans="1:2" ht="23.4">
       <c r="A26" s="11" t="s">
         <v>43</v>
       </c>
@@ -2757,7 +3114,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="23.25">
+    <row r="27" spans="1:2" ht="23.4">
       <c r="A27" s="11" t="s">
         <v>48</v>
       </c>
@@ -2776,13 +3133,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B59058-7D5E-48A2-8FB1-7D76323DAA63}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q27" sqref="A1:Q27"/>
+    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="16384" width="9.109375" style="41"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Alterações necessárias | Prof Gerson
</commit_message>
<xml_diff>
--- a/Análise de Sistemas/PBC - Product Backlog Classified V2.xlsx
+++ b/Análise de Sistemas/PBC - Product Backlog Classified V2.xlsx
@@ -1,33 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.nascimento\Desktop\Grupo_04-2ADSA\Análise de Sistemas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Gp 4\Grupo_04-2ADSA\Análise de Sistemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C551E9CD-9A1F-4805-82FE-C5686B25EE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36810" yWindow="4215" windowWidth="12300" windowHeight="6150" tabRatio="350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36810" yWindow="4215" windowWidth="12300" windowHeight="6150" tabRatio="350" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
     <sheet name="Dados" sheetId="14" r:id="rId2"/>
     <sheet name="USER STORIE" sheetId="16" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Alexander Barreira</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{CDAF273E-A20B-4D5C-B0D1-B3564A967A64}">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{EE39FC19-3292-4006-90AF-BA8C8E76E8E0}">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -237,9 +236,6 @@
     <t>EXEMPLOS</t>
   </si>
   <si>
-    <t>A aplicação deverá estar integrada com o Slack</t>
-  </si>
-  <si>
     <t>Limpar o cache da máquina quando o nível de consumo de RAM, Memória ou Processamento estiver elevado durante várias leituras</t>
   </si>
   <si>
@@ -280,12 +276,15 @@
   </si>
   <si>
     <t>Após a reinicialização do sistema, os softwares necessarios para compras futuas devem ser iniciados de maneira automatica.</t>
+  </si>
+  <si>
+    <t>A aplicação deverá estar integrada com o Slack********</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -747,18 +746,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="20" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
@@ -1655,8 +1654,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>118382</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>39337</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>74083</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1671,8 +1670,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5003800" y="1427596"/>
-          <a:ext cx="4893582" cy="1310491"/>
+          <a:off x="5024967" y="1427596"/>
+          <a:ext cx="4914748" cy="2615237"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1745,7 +1744,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> Eu como técnico quero que o cache da máquina seja limpo quando o uso de processamento permaneça em um nível elevado durante um tempo prolongado.</a:t>
+            <a:t> Eu como técnico quero que o cache da máquina seja limpo quando o uso de processamento permaneça em um nível elevado durante um tempo prolongado. (coleta dos dados - CPU, MEMORIA, DISCO, armazenamento dos dados em banco, Métrica definida, API - Leitura de dados do cache, Funcionalidade de limpeza do cache)</a:t>
           </a:r>
           <a:endParaRPr lang="pt-BR" sz="1800">
             <a:effectLst/>
@@ -2392,44 +2391,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.5546875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="73.44140625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="0.6640625" style="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="14"/>
-    <col min="11" max="11" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="1.5703125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="73.42578125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="0.7109375" style="16" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="14"/>
+    <col min="11" max="11" width="13.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="8.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:11" ht="89.25" customHeight="1" thickBot="1">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
-    </row>
-    <row r="3" spans="2:11" ht="9.9" customHeight="1" thickBot="1"/>
-    <row r="4" spans="2:11" s="20" customFormat="1" ht="24.9" customHeight="1" thickBot="1">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
+    </row>
+    <row r="3" spans="2:11" ht="9.9499999999999993" customHeight="1" thickBot="1"/>
+    <row r="4" spans="2:11" s="20" customFormat="1" ht="24.95" customHeight="1" thickBot="1">
       <c r="B4" s="33" t="s">
         <v>23</v>
       </c>
@@ -2452,18 +2451,18 @@
         <v>13</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="24" customFormat="1" ht="29.4" thickBot="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="24" customFormat="1" ht="45.75" thickBot="1">
       <c r="B5" s="39" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="23" t="s">
@@ -2478,10 +2477,10 @@
         <v>21</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="23" t="s">
@@ -2491,15 +2490,15 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="2:11" s="24" customFormat="1" ht="29.4" thickBot="1">
+    <row r="7" spans="2:11" s="24" customFormat="1" ht="30.75" thickBot="1">
       <c r="B7" s="39" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="23" t="s">
@@ -2511,15 +2510,15 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
     </row>
-    <row r="8" spans="2:11" s="24" customFormat="1" ht="43.8" thickBot="1">
+    <row r="8" spans="2:11" s="24" customFormat="1" ht="45.75" thickBot="1">
       <c r="B8" s="39" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="23" t="s">
@@ -2529,15 +2528,15 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
     </row>
-    <row r="9" spans="2:11" s="24" customFormat="1" ht="29.4" thickBot="1">
+    <row r="9" spans="2:11" s="24" customFormat="1" ht="30.75" thickBot="1">
       <c r="B9" s="39" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="23" t="s">
@@ -2552,10 +2551,10 @@
         <v>21</v>
       </c>
       <c r="C10" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="37" t="s">
         <v>62</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>63</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="23" t="s">
@@ -2565,15 +2564,15 @@
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
     </row>
-    <row r="11" spans="2:11" s="24" customFormat="1" ht="49.2" customHeight="1" thickBot="1">
+    <row r="11" spans="2:11" s="24" customFormat="1" ht="49.15" customHeight="1" thickBot="1">
       <c r="B11" s="39" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="42" t="s">
         <v>64</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>65</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="23"/>
@@ -2889,7 +2888,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C4" location="Dados!A1" display="Artefato de Referência (XX#R)" xr:uid="{D05B6432-AA2C-4045-919C-377B36218316}"/>
+    <hyperlink ref="C4" location="Dados!A1" display="Artefato de Referência (XX#R)"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2898,13 +2897,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Dados!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>B5:B24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Dados!$A$14:$A$14</xm:f>
           </x14:formula1>
@@ -2917,19 +2916,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="52.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.88671875" style="2"/>
+    <col min="1" max="1" width="52.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1">
@@ -3034,7 +3033,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="23.4">
+    <row r="17" spans="1:2" ht="23.25">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="23.4">
+    <row r="18" spans="1:2" ht="23.25">
       <c r="A18" s="11" t="s">
         <v>26</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23.4">
+    <row r="19" spans="1:2" ht="23.25">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -3058,7 +3057,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="23.4">
+    <row r="20" spans="1:2" ht="23.25">
       <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
@@ -3066,7 +3065,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="23.4">
+    <row r="21" spans="1:2" ht="23.25">
       <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
@@ -3074,7 +3073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="23.4">
+    <row r="22" spans="1:2" ht="23.25">
       <c r="A22" s="11" t="s">
         <v>30</v>
       </c>
@@ -3082,7 +3081,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="23.4">
+    <row r="23" spans="1:2" ht="23.25">
       <c r="A23" s="11" t="s">
         <v>31</v>
       </c>
@@ -3090,7 +3089,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="23.4">
+    <row r="24" spans="1:2" ht="23.25">
       <c r="A24" s="11" t="s">
         <v>32</v>
       </c>
@@ -3098,7 +3097,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="23.4">
+    <row r="25" spans="1:2" ht="23.25">
       <c r="A25" s="11" t="s">
         <v>33</v>
       </c>
@@ -3106,7 +3105,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="23.4">
+    <row r="26" spans="1:2" ht="23.25">
       <c r="A26" s="11" t="s">
         <v>43</v>
       </c>
@@ -3114,7 +3113,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="23.4">
+    <row r="27" spans="1:2" ht="23.25">
       <c r="A27" s="11" t="s">
         <v>48</v>
       </c>
@@ -3130,16 +3129,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B59058-7D5E-48A2-8FB1-7D76323DAA63}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="41"/>
+    <col min="1" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Finalização dos US e product backlog
</commit_message>
<xml_diff>
--- a/Análise de Sistemas/PBC - Product Backlog Classified V2.xlsx
+++ b/Análise de Sistemas/PBC - Product Backlog Classified V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Guilherme\bandtec\Grupo de PI\Grupo_04-2ADSA\Análise de Sistemas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeto em Grupo (P.I)\Grupo_04-2ADSA\Análise de Sistemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D55E62-B397-49B6-9F74-C2244D233BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB73B733-5AFC-4C69-BE4F-C2C3F7839714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>João</t>
   </si>
@@ -246,18 +246,6 @@
     <t>A aplicação deverá monitorar o hardware das máquinas e mostrar as informações em uma DASHBOARD (SITE).</t>
   </si>
   <si>
-    <t>US#05 &lt;Verificação de transação&gt;</t>
-  </si>
-  <si>
-    <t>Realizar a verificação do sistema para saber se existe alguma transação em andamento no momento em que o totem estiver ligado.</t>
-  </si>
-  <si>
-    <t>US#06 &lt;Abertura automatica do programa&gt;</t>
-  </si>
-  <si>
-    <t>Após a reinicialização do sistema, os softwares necessarios para compras futuas devem ser iniciados de maneira automatica.</t>
-  </si>
-  <si>
     <t>Ter uma API que faça o registro dos dados de uso do processador, memória RAM e disco.</t>
   </si>
   <si>
@@ -273,9 +261,6 @@
     <t>US#1.3 &lt;Visualização&gt;</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Será definido métricas para a % de consumo de CPU, Disco e RAM de acordo com os dados coletados no US#01</t>
   </si>
   <si>
@@ -285,12 +270,6 @@
     <t>Criar uma forma de comunicação com o usuário</t>
   </si>
   <si>
-    <t>US#1.1 &lt;Coleta de Dados&gt;*******</t>
-  </si>
-  <si>
-    <t>US#2.1 &lt;Métricas&gt;*******</t>
-  </si>
-  <si>
     <t>Criaremos uma conexão com slack realizando as notificações ao técnico caso o consumo de CPU, Disco ou RAM não estejam adequados</t>
   </si>
   <si>
@@ -324,10 +303,55 @@
     <t>US#05 &lt;Verificar Transação&gt;</t>
   </si>
   <si>
-    <t>US#5.1 &lt;&gt;</t>
-  </si>
-  <si>
     <t>Dar possibilidade para o técnico poder saber se a máquina em questão está em utilização.</t>
+  </si>
+  <si>
+    <t>US#5.1 &lt;Verificação&gt;</t>
+  </si>
+  <si>
+    <t>US#1.1 &lt;Coleta de Dados&gt;</t>
+  </si>
+  <si>
+    <t>US#2.1 &lt;Métricas&gt;</t>
+  </si>
+  <si>
+    <t>US#5.1 &lt;Coleta de dados&gt;</t>
+  </si>
+  <si>
+    <t>Quando iniciado uma nova compra e o cliente clicar no botão de pagamento, irá alterar o atributo transação para "true", impedindo o sistema de reiniciar.</t>
+  </si>
+  <si>
+    <t>Coletar os dados da transação por meio de uma api</t>
+  </si>
+  <si>
+    <t>US#5.2 &lt;Visualização&gt;</t>
+  </si>
+  <si>
+    <t>US#6 &lt;Sugestão de solução&gt;</t>
+  </si>
+  <si>
+    <t>US#6.1 &lt;Coleta de dados&gt;</t>
+  </si>
+  <si>
+    <t>Mostrará na dashboard a situação atual da transação.</t>
+  </si>
+  <si>
+    <t>Coletar os dados dos hardwares para verificar e sugerir as trocas dos mesmos.</t>
+  </si>
+  <si>
+    <t>Por meio de uma api, coletar os dados dos hardwares.</t>
+  </si>
+  <si>
+    <t>US#6.2 &lt;Analise dos dados&gt;</t>
+  </si>
+  <si>
+    <t>Realizando uma analise com base nos dados coletados para descobrir se está havendo algum problema com os hardwares</t>
+  </si>
+  <si>
+    <t>US#6.3 &lt;Envio das sugestões&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Com bases nas coletas, seria encaminhado via email sugestões de produtos para maquina. </t>
   </si>
 </sst>
 </file>
@@ -337,7 +361,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -465,6 +489,12 @@
       <name val="Exo"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Exo"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -552,49 +582,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -609,21 +602,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -652,7 +630,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -671,144 +649,144 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="20" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="20" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
@@ -835,7 +813,71 @@
     <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="109">
+  <dxfs count="117">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFB661"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEFB661"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFC8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2084,119 +2126,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>375998</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38726</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>380079</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>90763</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CaixaDeTexto 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3C04892-1274-4EE0-B348-C9F7BCB96237}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4643198" y="4410701"/>
-          <a:ext cx="4880881" cy="1347437"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1800">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>US#05</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1800" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Eu como técnico quero poder monitorar se existe alguma transação no momento, para que no momento em que for realizada alguma ação, não interfira na compra do cliente.</a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1800">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="pt-BR" sz="1800"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>123732</xdr:rowOff>
@@ -2438,8 +2367,25 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1800">
+            <a:rPr lang="pt-BR" sz="2000">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -2448,10 +2394,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>US#06</a:t>
+            <a:t>US#05</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1800" baseline="0">
+            <a:rPr lang="pt-BR" sz="2000" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -2460,8 +2406,13 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> Eu como técnico quero que meu programa tenha a capacidade de realizar a abertura dos programas necessarios quando estiver inicializando para que o processo seja automatizado, sem necessidade de um técnico.</a:t>
+            <a:t> Eu como técnico quero poder monitorar se existe alguma transação no momento, para que no momento em que for realizada alguma ação, não interfira na compra do cliente.</a:t>
           </a:r>
+          <a:endParaRPr lang="pt-BR" sz="2000">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="pt-BR" sz="1800">
             <a:effectLst/>
           </a:endParaRPr>
@@ -2531,81 +2482,50 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="pt-BR" sz="1800"/>
-            <a:t>US#07</a:t>
+            <a:t>US#06</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="pt-BR" sz="1800" baseline="0"/>
-            <a:t> Eu como técnico que meu programa tenha a capacidade de realizar a abertura dos programas necessarios para que n</a:t>
+            <a:t> Eu como técnico quero receber sugestões de soluções de problemas que envolvam os hardwares da máquina, para aumentar a durabilidade da máquina</a:t>
           </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1800"/>
         </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>156845</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>123190</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>423333</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>16420</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CaixaDeTexto 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3510663-E886-4D72-9DC6-F19499EF71D7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9978178" y="5520690"/>
-          <a:ext cx="5790988" cy="1321980"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="pt-BR" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -3107,31 +3027,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K49"/>
+  <dimension ref="B1:L45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="23.15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="73.140625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="0.5703125" style="23" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="21"/>
-    <col min="11" max="11" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="21"/>
+    <col min="1" max="1" width="1.54296875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.81640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="73.1796875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="0.54296875" style="17" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="21.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" style="15"/>
+    <col min="11" max="11" width="13.7265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="8.25" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:11" ht="89.25" customHeight="1" thickBot="1">
-      <c r="B2" s="25" t="s">
+    <row r="1" spans="2:12" ht="8.25" customHeight="1"/>
+    <row r="2" spans="2:12" ht="89.25" customHeight="1">
+      <c r="B2" s="26" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="26"/>
@@ -3140,916 +3060,944 @@
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
-    </row>
-    <row r="3" spans="2:11" ht="9.9499999999999993" customHeight="1" thickBot="1"/>
-    <row r="4" spans="2:11" s="28" customFormat="1" ht="24.95" customHeight="1" thickBot="1">
-      <c r="B4" s="16" t="s">
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="2:12" ht="10" customHeight="1">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="2:12" s="19" customFormat="1" ht="25" customHeight="1">
+      <c r="B4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="31" customFormat="1" ht="30.75" thickBot="1">
-      <c r="B5" s="32" t="s">
+    <row r="5" spans="2:12" s="20" customFormat="1" ht="29">
+      <c r="B5" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="39"/>
+      <c r="F5" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+    </row>
+    <row r="6" spans="2:12" s="20" customFormat="1" ht="29">
+      <c r="B6" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+    </row>
+    <row r="7" spans="2:12" s="20" customFormat="1" ht="29">
+      <c r="B7" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+    </row>
+    <row r="8" spans="2:12" s="20" customFormat="1" ht="29">
+      <c r="B8" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+    </row>
+    <row r="9" spans="2:12" s="20" customFormat="1" ht="6.75" customHeight="1">
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+    </row>
+    <row r="10" spans="2:12" s="20" customFormat="1" ht="22.5" customHeight="1">
+      <c r="B10" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="46"/>
+      <c r="F10" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+    </row>
+    <row r="11" spans="2:12" s="20" customFormat="1" ht="29">
+      <c r="B11" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="2:12" s="20" customFormat="1" ht="43.5">
+      <c r="B12" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+    </row>
+    <row r="13" spans="2:12" s="20" customFormat="1" ht="6.75" customHeight="1">
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="14" spans="2:12" s="20" customFormat="1" ht="29">
+      <c r="B14" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+    </row>
+    <row r="15" spans="2:12" s="20" customFormat="1" ht="29">
+      <c r="B15" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="39"/>
+      <c r="F15" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="25"/>
+    </row>
+    <row r="16" spans="2:12" s="20" customFormat="1" ht="6.75" customHeight="1">
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+    </row>
+    <row r="17" spans="2:9" s="20" customFormat="1" ht="14.5">
+      <c r="B17" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-    </row>
-    <row r="6" spans="2:11" s="31" customFormat="1" ht="30.75" thickBot="1">
-      <c r="B6" s="32" t="s">
+      <c r="E17" s="39"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+    </row>
+    <row r="18" spans="2:9" s="20" customFormat="1" ht="43.5">
+      <c r="B18" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-    </row>
-    <row r="7" spans="2:11" s="31" customFormat="1" ht="45.75" thickBot="1">
-      <c r="B7" s="32" t="s">
+      <c r="C18" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="39"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="2:9" s="20" customFormat="1" ht="6.75" customHeight="1">
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+    </row>
+    <row r="20" spans="2:9" s="20" customFormat="1" ht="29">
+      <c r="B20" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-    </row>
-    <row r="8" spans="2:11" s="31" customFormat="1" ht="30.75" thickBot="1">
-      <c r="B8" s="32" t="s">
+      <c r="C20" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="39"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+    </row>
+    <row r="21" spans="2:9" s="20" customFormat="1" ht="14.5">
+      <c r="B21" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-    </row>
-    <row r="9" spans="2:11" s="31" customFormat="1" ht="6.75" customHeight="1" thickBot="1">
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-    </row>
-    <row r="10" spans="2:11" s="31" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B10" s="32" t="s">
+      <c r="C21" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+    </row>
+    <row r="22" spans="2:9" s="20" customFormat="1" ht="43.5">
+      <c r="B22" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="35" t="s">
+      <c r="C22" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-    </row>
-    <row r="11" spans="2:11" s="31" customFormat="1" ht="30.75" thickBot="1">
-      <c r="B11" s="32" t="s">
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="2:9" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="B23" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-    </row>
-    <row r="12" spans="2:11" s="31" customFormat="1" ht="45.75" thickBot="1">
-      <c r="B12" s="32" t="s">
+      <c r="C23" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+    </row>
+    <row r="24" spans="2:9" s="20" customFormat="1" ht="6.75" customHeight="1">
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+    </row>
+    <row r="25" spans="2:9" s="20" customFormat="1" ht="29">
+      <c r="B25" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" spans="2:11" s="31" customFormat="1" ht="6.75" customHeight="1" thickBot="1">
-      <c r="B13" s="43"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-    </row>
-    <row r="14" spans="2:11" s="31" customFormat="1" ht="30.75" thickBot="1">
-      <c r="B14" s="32" t="s">
+      <c r="C25" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="40"/>
+    </row>
+    <row r="26" spans="2:9" s="20" customFormat="1" ht="45" customHeight="1">
+      <c r="B26" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" spans="2:11" s="31" customFormat="1" ht="45.75" thickBot="1">
-      <c r="B15" s="32" t="s">
+      <c r="C26" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="39"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="40"/>
+    </row>
+    <row r="27" spans="2:9" s="20" customFormat="1" ht="49.15" customHeight="1">
+      <c r="B27" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="2:11" s="31" customFormat="1" ht="6.75" customHeight="1" thickBot="1">
-      <c r="B16" s="43"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-    </row>
-    <row r="17" spans="2:9" s="31" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B17" s="32" t="s">
+      <c r="C27" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="39"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="40"/>
+    </row>
+    <row r="28" spans="2:9" s="20" customFormat="1" ht="29">
+      <c r="B28" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="18" spans="2:9" s="31" customFormat="1" ht="60.75" thickBot="1">
-      <c r="B18" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-    </row>
-    <row r="19" spans="2:9" s="31" customFormat="1" ht="6.75" customHeight="1" thickBot="1">
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-    </row>
-    <row r="20" spans="2:9" s="31" customFormat="1" ht="30.75" thickBot="1">
-      <c r="B20" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-    </row>
-    <row r="21" spans="2:9" s="31" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B21" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-    </row>
-    <row r="22" spans="2:9" s="31" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B22" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-    </row>
-    <row r="23" spans="2:9" s="31" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B23" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-    </row>
-    <row r="24" spans="2:9" s="31" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B24" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="35" t="s">
+      <c r="C28" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="46"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-    </row>
-    <row r="25" spans="2:9" s="31" customFormat="1" ht="45" customHeight="1" thickBot="1">
-      <c r="B25" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-    </row>
-    <row r="26" spans="2:9" s="31" customFormat="1" ht="49.15" customHeight="1" thickBot="1">
-      <c r="B26" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="35"/>
-    </row>
-    <row r="27" spans="2:9" s="31" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B27" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-    </row>
-    <row r="28" spans="2:9" s="31" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B28" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-    </row>
-    <row r="29" spans="2:9" s="31" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B29" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-    </row>
-    <row r="30" spans="2:9" s="31" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B30" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-    </row>
-    <row r="31" spans="2:9" s="31" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B31" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-    </row>
-    <row r="32" spans="2:9" s="31" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
-      <c r="B32" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-    </row>
-    <row r="33" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="G33" s="42"/>
-    </row>
-    <row r="34" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="G34" s="42"/>
-    </row>
-    <row r="35" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C35" s="40"/>
-      <c r="E35" s="41"/>
-      <c r="G35" s="42"/>
-    </row>
-    <row r="36" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="G36" s="42"/>
-    </row>
-    <row r="37" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C37" s="40"/>
-      <c r="E37" s="41"/>
-      <c r="G37" s="42"/>
-    </row>
-    <row r="38" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C38" s="40"/>
-      <c r="E38" s="41"/>
-      <c r="G38" s="42"/>
-    </row>
-    <row r="39" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C39" s="40"/>
-      <c r="E39" s="41"/>
-      <c r="G39" s="42"/>
-    </row>
-    <row r="40" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C40" s="40"/>
-      <c r="E40" s="41"/>
-      <c r="G40" s="42"/>
-    </row>
-    <row r="41" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C41" s="40"/>
-      <c r="E41" s="41"/>
-      <c r="G41" s="42"/>
-    </row>
-    <row r="42" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C42" s="40"/>
-      <c r="E42" s="41"/>
-      <c r="G42" s="42"/>
-    </row>
-    <row r="43" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C43" s="40"/>
-      <c r="E43" s="41"/>
-      <c r="G43" s="42"/>
-    </row>
-    <row r="44" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C44" s="40"/>
-      <c r="E44" s="41"/>
-      <c r="G44" s="42"/>
-    </row>
-    <row r="45" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C45" s="40"/>
-      <c r="E45" s="41"/>
-      <c r="G45" s="42"/>
-    </row>
-    <row r="46" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C46" s="40"/>
-      <c r="E46" s="41"/>
-      <c r="G46" s="42"/>
-    </row>
-    <row r="47" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C47" s="40"/>
-      <c r="E47" s="41"/>
-      <c r="G47" s="42"/>
-    </row>
-    <row r="48" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C48" s="40"/>
-      <c r="E48" s="41"/>
-      <c r="G48" s="42"/>
-    </row>
-    <row r="49" spans="3:7" s="31" customFormat="1" ht="23.1" customHeight="1">
-      <c r="C49" s="40"/>
-      <c r="E49" s="41"/>
-      <c r="G49" s="42"/>
+      <c r="I28" s="40"/>
+    </row>
+    <row r="29" spans="2:9" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C29" s="22"/>
+      <c r="E29" s="23"/>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="2:9" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C30" s="22"/>
+      <c r="E30" s="23"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="2:9" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C31" s="22"/>
+      <c r="E31" s="23"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="2:9" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C32" s="22"/>
+      <c r="E32" s="23"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C33" s="22"/>
+      <c r="E33" s="23"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C34" s="22"/>
+      <c r="E34" s="23"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C35" s="22"/>
+      <c r="E35" s="23"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C36" s="22"/>
+      <c r="E36" s="23"/>
+      <c r="G36" s="24"/>
+    </row>
+    <row r="37" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C37" s="22"/>
+      <c r="E37" s="23"/>
+      <c r="G37" s="24"/>
+    </row>
+    <row r="38" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C38" s="22"/>
+      <c r="E38" s="23"/>
+      <c r="G38" s="24"/>
+    </row>
+    <row r="39" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C39" s="22"/>
+      <c r="E39" s="23"/>
+      <c r="G39" s="24"/>
+    </row>
+    <row r="40" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C40" s="22"/>
+      <c r="E40" s="23"/>
+      <c r="G40" s="24"/>
+    </row>
+    <row r="41" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C41" s="22"/>
+      <c r="E41" s="23"/>
+      <c r="G41" s="24"/>
+    </row>
+    <row r="42" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C42" s="22"/>
+      <c r="E42" s="23"/>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C43" s="22"/>
+      <c r="E43" s="23"/>
+      <c r="G43" s="24"/>
+    </row>
+    <row r="44" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C44" s="22"/>
+      <c r="E44" s="23"/>
+      <c r="G44" s="24"/>
+    </row>
+    <row r="45" spans="3:7" s="20" customFormat="1" ht="23.15" customHeight="1">
+      <c r="C45" s="22"/>
+      <c r="E45" s="23"/>
+      <c r="G45" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:I2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="D29 B12:B13 D13 B17:B18 B20:B32">
-    <cfRule type="expression" dxfId="108" priority="185">
+  <conditionalFormatting sqref="D28 B12:B13 D13 B17:B18 B20:B23 B25:B28">
+    <cfRule type="expression" dxfId="116" priority="201">
       <formula>$B12="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="186">
+    <cfRule type="expression" dxfId="115" priority="202">
       <formula>$B12="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="187">
+    <cfRule type="expression" dxfId="114" priority="203">
       <formula>$B12="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="188">
+    <cfRule type="expression" dxfId="113" priority="204">
       <formula>$B12="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8 C11:C13 C15 C17:C18 C20:C32">
-    <cfRule type="expression" dxfId="104" priority="161">
+  <conditionalFormatting sqref="C8 C11:C13 C15 C17:C18 C20:C23 C25:C26 C28">
+    <cfRule type="expression" dxfId="112" priority="177">
       <formula>$B8="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="162">
+    <cfRule type="expression" dxfId="111" priority="178">
       <formula>$B8="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="163">
+    <cfRule type="expression" dxfId="110" priority="179">
       <formula>$B8="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="164">
+    <cfRule type="expression" dxfId="109" priority="180">
       <formula>$B8="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8 D11:D12 D30:D32 D15 D17:D18 D20:D28">
-    <cfRule type="expression" dxfId="100" priority="152">
+  <conditionalFormatting sqref="D8 D11:D12 D15 D17:D18 D20:D23 D25:D27">
+    <cfRule type="expression" dxfId="108" priority="168">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="157">
+    <cfRule type="expression" dxfId="107" priority="173">
       <formula>$B8="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="158">
+    <cfRule type="expression" dxfId="106" priority="174">
       <formula>$B8="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="159">
+    <cfRule type="expression" dxfId="105" priority="175">
       <formula>$B8="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="160">
+    <cfRule type="expression" dxfId="104" priority="176">
       <formula>$B8="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="95" priority="135">
+    <cfRule type="expression" dxfId="103" priority="151">
       <formula>$B5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="136">
+    <cfRule type="expression" dxfId="102" priority="152">
       <formula>$B5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="137">
+    <cfRule type="expression" dxfId="101" priority="153">
       <formula>$B5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="138">
+    <cfRule type="expression" dxfId="100" priority="154">
       <formula>$B5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="91" priority="131">
+    <cfRule type="expression" dxfId="99" priority="147">
       <formula>$B5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="132">
+    <cfRule type="expression" dxfId="98" priority="148">
       <formula>$B5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="133">
+    <cfRule type="expression" dxfId="97" priority="149">
       <formula>$B5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="134">
+    <cfRule type="expression" dxfId="96" priority="150">
       <formula>$B5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="87" priority="91">
+    <cfRule type="expression" dxfId="95" priority="107">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="92">
+    <cfRule type="expression" dxfId="94" priority="108">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="93">
+    <cfRule type="expression" dxfId="93" priority="109">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="94">
+    <cfRule type="expression" dxfId="92" priority="110">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="95">
+    <cfRule type="expression" dxfId="91" priority="111">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="82" priority="121">
+    <cfRule type="expression" dxfId="90" priority="137">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="122">
+    <cfRule type="expression" dxfId="89" priority="138">
       <formula>$B5="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="123">
+    <cfRule type="expression" dxfId="88" priority="139">
       <formula>$B5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="124">
+    <cfRule type="expression" dxfId="87" priority="140">
       <formula>$B5="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="125">
+    <cfRule type="expression" dxfId="86" priority="141">
       <formula>$B5="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="77" priority="117">
+    <cfRule type="expression" dxfId="85" priority="133">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="118">
+    <cfRule type="expression" dxfId="84" priority="134">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="119">
+    <cfRule type="expression" dxfId="83" priority="135">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="120">
+    <cfRule type="expression" dxfId="82" priority="136">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="73" priority="113">
+    <cfRule type="expression" dxfId="81" priority="129">
       <formula>$B8="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="114">
+    <cfRule type="expression" dxfId="80" priority="130">
       <formula>$B8="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="115">
+    <cfRule type="expression" dxfId="79" priority="131">
       <formula>$B8="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="116">
+    <cfRule type="expression" dxfId="78" priority="132">
       <formula>$B8="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="69" priority="109">
+    <cfRule type="expression" dxfId="77" priority="125">
       <formula>$B6="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="110">
+    <cfRule type="expression" dxfId="76" priority="126">
       <formula>$B6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="111">
+    <cfRule type="expression" dxfId="75" priority="127">
       <formula>$B6="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="112">
+    <cfRule type="expression" dxfId="74" priority="128">
       <formula>$B6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="65" priority="105">
+    <cfRule type="expression" dxfId="73" priority="121">
       <formula>$B6="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="106">
+    <cfRule type="expression" dxfId="72" priority="122">
       <formula>$B6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="107">
+    <cfRule type="expression" dxfId="71" priority="123">
       <formula>$B6="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="108">
+    <cfRule type="expression" dxfId="70" priority="124">
       <formula>$B6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="61" priority="100">
+    <cfRule type="expression" dxfId="69" priority="116">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="101">
+    <cfRule type="expression" dxfId="68" priority="117">
       <formula>$B6="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="102">
+    <cfRule type="expression" dxfId="67" priority="118">
       <formula>$B6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="103">
+    <cfRule type="expression" dxfId="66" priority="119">
       <formula>$B6="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="104">
+    <cfRule type="expression" dxfId="65" priority="120">
       <formula>$B6="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="56" priority="96">
+    <cfRule type="expression" dxfId="64" priority="112">
       <formula>$B7="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="97">
+    <cfRule type="expression" dxfId="63" priority="113">
       <formula>$B7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="98">
+    <cfRule type="expression" dxfId="62" priority="114">
       <formula>$B7="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="99">
+    <cfRule type="expression" dxfId="61" priority="115">
       <formula>$B7="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9 D9">
-    <cfRule type="expression" dxfId="52" priority="87">
+    <cfRule type="expression" dxfId="60" priority="103">
       <formula>$B9="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="88">
+    <cfRule type="expression" dxfId="59" priority="104">
       <formula>$B9="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="89">
+    <cfRule type="expression" dxfId="58" priority="105">
       <formula>$B9="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="90">
+    <cfRule type="expression" dxfId="57" priority="106">
       <formula>$B9="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="48" priority="71">
+    <cfRule type="expression" dxfId="56" priority="87">
       <formula>$B9="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="72">
+    <cfRule type="expression" dxfId="55" priority="88">
       <formula>$B9="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="73">
+    <cfRule type="expression" dxfId="54" priority="89">
       <formula>$B9="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="74">
+    <cfRule type="expression" dxfId="53" priority="90">
       <formula>$B9="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10 D10">
-    <cfRule type="expression" dxfId="44" priority="79">
+    <cfRule type="expression" dxfId="52" priority="95">
       <formula>$B10="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="80">
+    <cfRule type="expression" dxfId="51" priority="96">
       <formula>$B10="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="81">
+    <cfRule type="expression" dxfId="50" priority="97">
       <formula>$B10="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="82">
+    <cfRule type="expression" dxfId="49" priority="98">
       <formula>$B10="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="40" priority="75">
+    <cfRule type="expression" dxfId="48" priority="91">
       <formula>$B10="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="76">
+    <cfRule type="expression" dxfId="47" priority="92">
       <formula>$B10="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="77">
+    <cfRule type="expression" dxfId="46" priority="93">
       <formula>$B10="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="78">
+    <cfRule type="expression" dxfId="45" priority="94">
       <formula>$B10="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="36" priority="67">
+    <cfRule type="expression" dxfId="44" priority="83">
       <formula>$B11="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="68">
+    <cfRule type="expression" dxfId="43" priority="84">
       <formula>$B11="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="69">
+    <cfRule type="expression" dxfId="42" priority="85">
       <formula>$B11="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="70">
+    <cfRule type="expression" dxfId="41" priority="86">
       <formula>$B11="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="32" priority="30">
+    <cfRule type="expression" dxfId="40" priority="46">
       <formula>$B14="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="31">
+    <cfRule type="expression" dxfId="39" priority="47">
       <formula>$B14="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="32">
+    <cfRule type="expression" dxfId="38" priority="48">
       <formula>$B14="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="33">
+    <cfRule type="expression" dxfId="37" priority="49">
       <formula>$B14="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="28" priority="26">
+    <cfRule type="expression" dxfId="36" priority="42">
       <formula>$B14="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27">
+    <cfRule type="expression" dxfId="35" priority="43">
       <formula>$B14="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28">
+    <cfRule type="expression" dxfId="34" priority="44">
       <formula>$B14="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29">
+    <cfRule type="expression" dxfId="33" priority="45">
       <formula>$B14="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="24" priority="21">
+    <cfRule type="expression" dxfId="32" priority="37">
       <formula>$B$4="Plannedd"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="22">
+    <cfRule type="expression" dxfId="31" priority="38">
       <formula>$B14="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="30" priority="39">
       <formula>$B14="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="24">
+    <cfRule type="expression" dxfId="29" priority="40">
       <formula>$B14="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="25">
+    <cfRule type="expression" dxfId="28" priority="41">
       <formula>$B14="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="19" priority="17">
+    <cfRule type="expression" dxfId="27" priority="33">
       <formula>$B15="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
+    <cfRule type="expression" dxfId="26" priority="34">
       <formula>$B15="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="25" priority="35">
       <formula>$B15="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="24" priority="36">
       <formula>$B15="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16 D16">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="23" priority="29">
       <formula>$B16="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="22" priority="30">
       <formula>$B16="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="21" priority="31">
       <formula>$B16="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>$B16="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="19" priority="25">
       <formula>$B16="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>$B16="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="17" priority="27">
       <formula>$B16="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="16" priority="28">
       <formula>$B16="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19 D19">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="15" priority="21">
       <formula>$B19="Done!"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="14" priority="22">
       <formula>$B19="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="13" priority="23">
       <formula>$B19="Blocked"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="12" priority="24">
       <formula>$B19="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="11" priority="17">
+      <formula>$B19="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="18">
+      <formula>$B19="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="19">
+      <formula>$B19="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="20">
+      <formula>$B19="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24 D24">
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>$B24="Done!"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>$B24="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>$B24="Blocked"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>$B24="Dropped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$B19="Done!"</formula>
+      <formula>$B24="Done!"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$B19="Ongoing"</formula>
+      <formula>$B24="Ongoing"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$B19="Blocked"</formula>
+      <formula>$B24="Blocked"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$B19="Dropped"</formula>
+      <formula>$B24="Dropped"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -4066,13 +4014,13 @@
           <x14:formula1>
             <xm:f>Dados!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B32</xm:sqref>
+          <xm:sqref>B5:B28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Dados!$A$14:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E5:E32</xm:sqref>
+          <xm:sqref>E5:E28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4084,16 +4032,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A9" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="18"/>
-    <col min="7" max="7" width="7.140625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="6" width="9.1796875" style="14"/>
+    <col min="7" max="7" width="7.1796875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" style="14" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="14"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4105,16 +4053,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="52.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="52.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1">
@@ -4219,7 +4167,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="23.25">
+    <row r="17" spans="1:2" ht="23.5">
       <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
@@ -4227,7 +4175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="23.25">
+    <row r="18" spans="1:2" ht="23.5">
       <c r="A18" s="11" t="s">
         <v>26</v>
       </c>
@@ -4235,7 +4183,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23.25">
+    <row r="19" spans="1:2" ht="23.5">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -4243,7 +4191,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="23.25">
+    <row r="20" spans="1:2" ht="23.5">
       <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
@@ -4251,7 +4199,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="23.25">
+    <row r="21" spans="1:2" ht="23.5">
       <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
@@ -4259,7 +4207,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="23.25">
+    <row r="22" spans="1:2" ht="23.5">
       <c r="A22" s="11" t="s">
         <v>30</v>
       </c>
@@ -4267,7 +4215,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="23.25">
+    <row r="23" spans="1:2" ht="23.5">
       <c r="A23" s="11" t="s">
         <v>31</v>
       </c>
@@ -4275,7 +4223,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="23.25">
+    <row r="24" spans="1:2" ht="23.5">
       <c r="A24" s="11" t="s">
         <v>32</v>
       </c>
@@ -4283,7 +4231,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="23.25">
+    <row r="25" spans="1:2" ht="23.5">
       <c r="A25" s="11" t="s">
         <v>33</v>
       </c>
@@ -4291,7 +4239,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="23.25">
+    <row r="26" spans="1:2" ht="23.5">
       <c r="A26" s="11" t="s">
         <v>43</v>
       </c>
@@ -4299,7 +4247,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="23.25">
+    <row r="27" spans="1:2" ht="23.5">
       <c r="A27" s="11" t="s">
         <v>48</v>
       </c>

</xml_diff>